<commit_message>
Modify: Modified some selected options and handled some error cases.
</commit_message>
<xml_diff>
--- a/libs/fuel-xpert/src/components/FileUpload/FuelExpert.xlsx
+++ b/libs/fuel-xpert/src/components/FileUpload/FuelExpert.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/praveen/Documents/GitHub/IDC/Projects/tu-fuel-insight/libs/fuel-xpert/src/components/FileUpload/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\idcuser\trackunit-projects\tu-fuel-insight\libs\fuel-xpert\src\components\FileUpload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08846795-71F2-8D47-B957-27BFBA75F228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0646EEBD-49FC-49BA-A792-28F1DDD366E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="500" windowWidth="28800" windowHeight="20080" xr2:uid="{A3BF28FF-B55C-4A49-963F-40F408DB3A5A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A3BF28FF-B55C-4A49-963F-40F408DB3A5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Color</t>
   </si>
   <si>
-    <t>BorderColor</t>
-  </si>
-  <si>
     <t>Timestamp</t>
   </si>
   <si>
@@ -84,13 +81,16 @@
   </si>
   <si>
     <t>Vehicle 2</t>
+  </si>
+  <si>
+    <t>TextColor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,14 +172,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -518,19 +517,19 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,36 +540,36 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="20.25">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3">
         <v>45505.333333333336</v>
@@ -579,7 +578,7 @@
         <v>2000</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="4">
         <v>30</v>
@@ -588,18 +587,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="20.25">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3">
         <v>45506.333333333336</v>
@@ -608,7 +607,7 @@
         <v>2000</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" s="4">
         <v>22</v>
@@ -617,18 +616,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="20.25">
       <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3">
         <v>45507.333333333336</v>
@@ -637,7 +636,7 @@
         <v>2000</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="4">
         <v>88</v>
@@ -646,18 +645,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="20.25">
       <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
         <v>45508.333333333336</v>
@@ -666,7 +665,7 @@
         <v>5000</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="4">
         <v>50</v>
@@ -675,18 +674,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="20.25">
       <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3">
         <v>45509.333333333336</v>
@@ -695,7 +694,7 @@
         <v>2000</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="4">
         <v>30</v>
@@ -704,18 +703,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="20.25">
       <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="3">
         <v>45510.333333333336</v>
@@ -724,7 +723,7 @@
         <v>1000</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="4">
         <v>62</v>
@@ -733,18 +732,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="20.25">
       <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="3">
         <v>45511.333333333336</v>
@@ -753,7 +752,7 @@
         <v>2000</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="4">
         <v>45</v>
@@ -762,18 +761,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="20.25">
       <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" s="3">
         <v>45512.333333333336</v>
@@ -782,7 +781,7 @@
         <v>2000</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="4">
         <v>30</v>
@@ -791,18 +790,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="20.25">
       <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="3">
         <v>45513.333333333336</v>
@@ -811,7 +810,7 @@
         <v>2000</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H10" s="4">
         <v>30</v>
@@ -820,18 +819,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="20.25">
       <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="3">
         <v>45514.333333333336</v>
@@ -840,7 +839,7 @@
         <v>3000</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="4">
         <v>66</v>
@@ -849,18 +848,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="20.25">
       <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="3">
         <v>45515.333333333336</v>
@@ -869,7 +868,7 @@
         <v>2000</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" s="4">
         <v>30</v>
@@ -878,18 +877,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="20.25">
       <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="3">
         <v>45516.333333333336</v>
@@ -898,7 +897,7 @@
         <v>2000</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" s="4">
         <v>22</v>
@@ -907,18 +906,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="20.25">
       <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="3">
         <v>45517.333333333336</v>
@@ -927,7 +926,7 @@
         <v>2000</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" s="4">
         <v>88</v>
@@ -936,18 +935,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="20.25">
       <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" s="3">
         <v>45518.333333333336</v>
@@ -956,7 +955,7 @@
         <v>5000</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" s="4">
         <v>50</v>
@@ -965,18 +964,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="20.25">
       <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16" s="3">
         <v>45519.333333333336</v>
@@ -985,7 +984,7 @@
         <v>2000</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" s="4">
         <v>30</v>
@@ -994,18 +993,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="20.25">
       <c r="A17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="3">
         <v>45520.333333333336</v>
@@ -1014,7 +1013,7 @@
         <v>1000</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" s="4">
         <v>62</v>
@@ -1023,18 +1022,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="20.25">
       <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="3">
         <v>45521.333333333336</v>
@@ -1043,7 +1042,7 @@
         <v>2000</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" s="4">
         <v>45</v>
@@ -1052,18 +1051,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="20.25">
       <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="3">
         <v>45522.333333333336</v>
@@ -1072,7 +1071,7 @@
         <v>2000</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H19" s="4">
         <v>30</v>
@@ -1081,18 +1080,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="20.25">
       <c r="A20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20" s="3">
         <v>45523.333333333336</v>
@@ -1101,7 +1100,7 @@
         <v>2000</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" s="4">
         <v>30</v>
@@ -1110,18 +1109,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="20.25">
       <c r="A21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" s="3">
         <v>45524.333333333336</v>
@@ -1130,7 +1129,7 @@
         <v>3000</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" s="4">
         <v>66</v>

</xml_diff>

<commit_message>
Modify: added new chnages
</commit_message>
<xml_diff>
--- a/libs/fuel-xpert/src/components/FileUpload/FuelExpert.xlsx
+++ b/libs/fuel-xpert/src/components/FileUpload/FuelExpert.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\idcuser\trackunit-projects\tu-fuel-insight\libs\fuel-xpert\src\components\FileUpload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/Development/trackunit/idc-workspace/libs/fuel-xpert/src/components/FileUpload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0646EEBD-49FC-49BA-A792-28F1DDD366E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E265AF-B550-D242-99BB-2E4AC5F5424D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A3BF28FF-B55C-4A49-963F-40F408DB3A5A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{A3BF28FF-B55C-4A49-963F-40F408DB3A5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -517,19 +517,19 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="20.25">
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -587,7 +587,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="20.25">
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -613,10 +613,10 @@
         <v>22</v>
       </c>
       <c r="I3" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="20.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -642,10 +642,10 @@
         <v>88</v>
       </c>
       <c r="I4" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="20.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -671,10 +671,10 @@
         <v>50</v>
       </c>
       <c r="I5" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="20.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -700,10 +700,10 @@
         <v>30</v>
       </c>
       <c r="I6" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="20.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -729,10 +729,10 @@
         <v>62</v>
       </c>
       <c r="I7" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="20.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -758,10 +758,10 @@
         <v>45</v>
       </c>
       <c r="I8" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="20.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -787,10 +787,10 @@
         <v>30</v>
       </c>
       <c r="I9" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="20.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -816,10 +816,10 @@
         <v>30</v>
       </c>
       <c r="I10" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="20.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -845,10 +845,10 @@
         <v>66</v>
       </c>
       <c r="I11" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="20.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -874,10 +874,10 @@
         <v>30</v>
       </c>
       <c r="I12" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="20.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -903,10 +903,10 @@
         <v>22</v>
       </c>
       <c r="I13" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="20.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -932,10 +932,10 @@
         <v>88</v>
       </c>
       <c r="I14" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="20.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -961,10 +961,10 @@
         <v>50</v>
       </c>
       <c r="I15" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="20.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -990,10 +990,10 @@
         <v>30</v>
       </c>
       <c r="I16" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="20.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1019,10 +1019,10 @@
         <v>62</v>
       </c>
       <c r="I17" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="20.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -1048,10 +1048,10 @@
         <v>45</v>
       </c>
       <c r="I18" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="20.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -1077,10 +1077,10 @@
         <v>30</v>
       </c>
       <c r="I19" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="20.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -1106,10 +1106,10 @@
         <v>30</v>
       </c>
       <c r="I20" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="20.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>66</v>
       </c>
       <c r="I21" s="4">
-        <v>25</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>